<commit_message>
Fixed lab1 and lab2 with license data for clients
</commit_message>
<xml_diff>
--- a/lr2/files/processed/etl_result.xlsx
+++ b/lr2/files/processed/etl_result.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="86">
   <si>
     <t>emp_num</t>
   </si>
@@ -79,16 +79,31 @@
     <t>паспорт</t>
   </si>
   <si>
-    <t>3417567187125683</t>
-  </si>
-  <si>
-    <t>4608599988123646</t>
-  </si>
-  <si>
-    <t>6714467987134587</t>
-  </si>
-  <si>
-    <t>5714567899129078</t>
+    <t>вод_удостоверение</t>
+  </si>
+  <si>
+    <t>3417567187</t>
+  </si>
+  <si>
+    <t>4608599988</t>
+  </si>
+  <si>
+    <t>6714467987</t>
+  </si>
+  <si>
+    <t>5714567899</t>
+  </si>
+  <si>
+    <t>125683</t>
+  </si>
+  <si>
+    <t>123646</t>
+  </si>
+  <si>
+    <t>134587</t>
+  </si>
+  <si>
+    <t>129078</t>
   </si>
   <si>
     <t>Сергеев</t>
@@ -719,13 +734,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -733,81 +748,96 @@
         <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -825,7 +855,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -833,7 +863,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -841,7 +871,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -849,7 +879,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -873,10 +903,10 @@
         <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -884,7 +914,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -895,7 +925,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -906,7 +936,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -917,7 +947,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -938,21 +968,21 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -960,10 +990,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -971,10 +1001,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -982,10 +1012,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -1006,7 +1036,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -1014,7 +1044,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1022,7 +1052,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1030,7 +1060,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1038,7 +1068,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1046,7 +1076,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -1054,7 +1084,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -1062,7 +1092,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -1070,7 +1100,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -1078,7 +1108,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1086,7 +1116,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -1094,7 +1124,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -1102,7 +1132,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -1110,7 +1140,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -1134,25 +1164,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1166,13 +1196,13 @@
         <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G2">
         <v>1500</v>
@@ -1189,13 +1219,13 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F3" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G3">
         <v>300</v>
@@ -1212,13 +1242,13 @@
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G4">
         <v>300</v>
@@ -1235,13 +1265,13 @@
         <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F5" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G5">
         <v>900</v>
@@ -1258,13 +1288,13 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="G6">
         <v>200</v>
@@ -1281,13 +1311,13 @@
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F7" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G7">
         <v>4500</v>
@@ -1304,13 +1334,13 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F8" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="G8">
         <v>600</v>
@@ -1327,13 +1357,13 @@
         <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G9">
         <v>1500</v>
@@ -1350,13 +1380,13 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F10" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G10">
         <v>300</v>
@@ -1373,13 +1403,13 @@
         <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F11" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G11">
         <v>400</v>
@@ -1396,13 +1426,13 @@
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E12" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F12" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G12">
         <v>250</v>
@@ -1419,13 +1449,13 @@
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F13" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G13">
         <v>700</v>
@@ -1442,13 +1472,13 @@
         <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F14" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G14">
         <v>311</v>
@@ -1465,13 +1495,13 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E15" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="F15" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G15">
         <v>300</v>
@@ -1488,13 +1518,13 @@
         <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E16" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="F16" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G16">
         <v>300</v>
@@ -1511,13 +1541,13 @@
         <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E17" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="F17" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G17">
         <v>700</v>
@@ -1534,13 +1564,13 @@
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E18" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="F18" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G18">
         <v>1200</v>

</xml_diff>